<commit_message>
Season up to 1/17
</commit_message>
<xml_diff>
--- a/data/CurrentSeason/ATL.xlsx
+++ b/data/CurrentSeason/ATL.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2851,6 +2851,67 @@
       </c>
       <c r="S39" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>45306</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>109</v>
+      </c>
+      <c r="E40" t="n">
+        <v>105.1</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G40" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="H40" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.172</v>
+      </c>
+      <c r="J40" t="n">
+        <v>103.7</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="L40" t="n">
+        <v>99</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.458</v>
+      </c>
+      <c r="N40" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="O40" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>94.2</v>
+      </c>
+      <c r="R40" t="n">
+        <v>1</v>
+      </c>
+      <c r="S40" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2864,7 +2925,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2891,11 +2952,11 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45306</v>
+        <v>45308</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -2904,50 +2965,50 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45308</v>
+        <v>45310</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45310</v>
+        <v>45311</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45311</v>
+        <v>45313</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45313</v>
+        <v>45315</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -2956,24 +3017,24 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45315</v>
+        <v>45317</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45317</v>
+        <v>45319</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -2982,11 +3043,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45319</v>
+        <v>45321</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -2995,11 +3056,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45321</v>
+        <v>45324</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>PHO</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -3008,11 +3069,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45324</v>
+        <v>45325</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PHO</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -3021,11 +3082,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45325</v>
+        <v>45327</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -3034,24 +3095,24 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -3060,24 +3121,24 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45331</v>
+        <v>45332</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45332</v>
+        <v>45334</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -3086,37 +3147,37 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45334</v>
+        <v>45336</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>CHO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45336</v>
+        <v>45345</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CHO</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45345</v>
+        <v>45347</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -3125,11 +3186,11 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45347</v>
+        <v>45349</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -3138,20 +3199,20 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45349</v>
+        <v>45351</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>BRK</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45351</v>
+        <v>45353</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -3164,11 +3225,11 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45353</v>
+        <v>45356</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BRK</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -3177,63 +3238,63 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45356</v>
+        <v>45357</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45357</v>
+        <v>45359</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45359</v>
+        <v>45361</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45361</v>
+        <v>45364</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45364</v>
+        <v>45366</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -3242,11 +3303,11 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -3255,11 +3316,11 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -3268,11 +3329,11 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45369</v>
+        <v>45372</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>PHO</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -3281,24 +3342,24 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45372</v>
+        <v>45374</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>PHO</t>
+          <t>CHO</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45374</v>
+        <v>45376</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>CHO</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -3307,11 +3368,11 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45376</v>
+        <v>45378</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -3320,11 +3381,11 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -3333,11 +3394,11 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45379</v>
+        <v>45381</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -3346,50 +3407,50 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45381</v>
+        <v>45383</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45383</v>
+        <v>45385</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45385</v>
+        <v>45387</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45387</v>
+        <v>45388</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -3398,24 +3459,24 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45388</v>
+        <v>45391</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45391</v>
+        <v>45392</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>CHO</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -3424,40 +3485,27 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45392</v>
+        <v>45394</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>CHO</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45394</v>
+        <v>45396</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
-        <v>45396</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>IND</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>